<commit_message>
added Hamming code answers
</commit_message>
<xml_diff>
--- a/Summative06/Summative06.xlsx
+++ b/Summative06/Summative06.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mnscu-my.sharepoint.com/personal/wp8798rh_minnstate_edu/Documents/GitHub/eprof1/MIS452/Summative06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{DD16A31F-4BAC-4B48-93CF-E68A2FD7162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{114CF8B2-46AE-4850-AEE9-F0348F61D172}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{DD16A31F-4BAC-4B48-93CF-E68A2FD7162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92C17A3A-5F60-4D79-B5FC-DFF75CD4C13B}"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ParityBits" sheetId="3" r:id="rId1"/>
     <sheet name="ErrorTimeCalcs" sheetId="2" r:id="rId2"/>
     <sheet name="HammingCode_Error" sheetId="6" r:id="rId3"/>
-    <sheet name="HammingCode_CorrectError" sheetId="5" r:id="rId4"/>
-    <sheet name="P6-1 Dec2Bin" sheetId="7" r:id="rId5"/>
-    <sheet name="P6-2 Bin2Dec" sheetId="8" r:id="rId6"/>
-    <sheet name="P6-3 CIDR" sheetId="9" r:id="rId7"/>
-    <sheet name="P6-4 Prefix" sheetId="10" r:id="rId8"/>
+    <sheet name="HammingCode_Error-Answer" sheetId="11" r:id="rId4"/>
+    <sheet name="HammingCode_CorrectError" sheetId="5" r:id="rId5"/>
+    <sheet name="HammingCode_Corrected-Answer" sheetId="12" r:id="rId6"/>
+    <sheet name="P6-1 Dec2Bin" sheetId="7" r:id="rId7"/>
+    <sheet name="P6-2 Bin2Dec" sheetId="8" r:id="rId8"/>
+    <sheet name="P6-3 CIDR" sheetId="9" r:id="rId9"/>
+    <sheet name="P6-4 Prefix" sheetId="10" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
+    <definedName name="degree">'[2]CRC-Q16'!$C$1</definedName>
     <definedName name="SubnetMask">'[1]P6-3 CIDR'!$E$24:$F$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -82,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
   <si>
     <t>b12</t>
   </si>
@@ -526,6 +531,15 @@
   </si>
   <si>
     <t>Hosts</t>
+  </si>
+  <si>
+    <t>White, 5e, pages 194-196</t>
+  </si>
+  <si>
+    <t>Error?</t>
+  </si>
+  <si>
+    <t>If Error, which bit?</t>
   </si>
 </sst>
 </file>
@@ -1196,6 +1210,34 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="ParityBits_PasteValues_Easy"/>
+      <sheetName val="ParityBits_Random"/>
+      <sheetName val="CRC-Q16"/>
+      <sheetName val="HammingCode_Error-Q14"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="C1">
+            <v>16</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Paulson, Patrick G" id="{907C4DD5-CAA1-474F-B138-1F9EA579D379}" userId="S::wp8798rh@minnstate.edu::b0df62ef-2774-4648-a1b3-1c1d265090a6" providerId="AD"/>
@@ -1505,17 +1547,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>28</v>
       </c>
@@ -1536,7 +1578,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>0</v>
       </c>
@@ -1563,7 +1605,7 @@
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -1590,18 +1632,18 @@
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="20">
         <f t="shared" ref="B4:G19" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1609,29 +1651,29 @@
       </c>
       <c r="E4" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f t="shared" ref="A5:G34" ca="1" si="1">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c r="B5" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1643,11 +1685,11 @@
       </c>
       <c r="E5" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1658,22 +1700,22 @@
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="B6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1685,21 +1727,21 @@
       </c>
       <c r="G6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1711,7 +1753,7 @@
       </c>
       <c r="E7" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1726,14 +1768,14 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="B8" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1745,11 +1787,11 @@
       </c>
       <c r="E8" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1760,18 +1802,18 @@
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="B9" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1783,25 +1825,25 @@
       </c>
       <c r="F9" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="B10" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1809,33 +1851,33 @@
       </c>
       <c r="D10" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1847,7 +1889,7 @@
       </c>
       <c r="E11" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1855,14 +1897,14 @@
       </c>
       <c r="G11" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
@@ -1877,7 +1919,7 @@
       </c>
       <c r="D12" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1889,14 +1931,14 @@
       </c>
       <c r="G12" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
@@ -1907,11 +1949,11 @@
       </c>
       <c r="C13" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1919,7 +1961,7 @@
       </c>
       <c r="F13" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1930,14 +1972,14 @@
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="B14" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1945,7 +1987,7 @@
       </c>
       <c r="D14" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1953,7 +1995,7 @@
       </c>
       <c r="F14" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1964,18 +2006,18 @@
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -1991,14 +2033,14 @@
       </c>
       <c r="G15" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
@@ -2017,7 +2059,7 @@
       </c>
       <c r="E16" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -2032,7 +2074,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
@@ -2043,7 +2085,7 @@
       </c>
       <c r="C17" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -2066,10 +2108,10 @@
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -2077,33 +2119,33 @@
       </c>
       <c r="C18" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -2111,15 +2153,15 @@
       </c>
       <c r="C19" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="20">
         <f t="shared" ca="1" si="0"/>
@@ -2127,17 +2169,17 @@
       </c>
       <c r="G19" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2157,7 +2199,7 @@
       </c>
       <c r="F20" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2168,26 +2210,26 @@
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2195,37 +2237,37 @@
       </c>
       <c r="G21" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2236,7 +2278,7 @@
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
@@ -2255,7 +2297,7 @@
       </c>
       <c r="E23" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2263,21 +2305,21 @@
       </c>
       <c r="G23" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2285,11 +2327,11 @@
       </c>
       <c r="D24" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2297,17 +2339,17 @@
       </c>
       <c r="G24" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2315,7 +2357,7 @@
       </c>
       <c r="C25" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2323,11 +2365,11 @@
       </c>
       <c r="E25" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2338,14 +2380,14 @@
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2357,11 +2399,11 @@
       </c>
       <c r="E26" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2372,14 +2414,14 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="B27" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2387,7 +2429,7 @@
       </c>
       <c r="D27" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2399,25 +2441,25 @@
       </c>
       <c r="G27" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="B28" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2425,11 +2467,11 @@
       </c>
       <c r="E28" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2440,10 +2482,10 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2455,7 +2497,7 @@
       </c>
       <c r="D29" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2463,7 +2505,7 @@
       </c>
       <c r="F29" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2474,7 +2516,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
@@ -2485,15 +2527,15 @@
       </c>
       <c r="C30" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2508,10 +2550,10 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2535,21 +2577,21 @@
       </c>
       <c r="G31" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="B32" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2557,33 +2599,33 @@
       </c>
       <c r="D32" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="B33" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2591,29 +2633,29 @@
       </c>
       <c r="D33" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2621,7 +2663,7 @@
       </c>
       <c r="C34" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2629,7 +2671,7 @@
       </c>
       <c r="E34" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="20">
         <f t="shared" ca="1" si="1"/>
@@ -2645,10 +2687,808 @@
       <c r="K34" s="19"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B349E9EF-46A3-44BF-ADBB-8103E35728F3}">
+  <dimension ref="A1:G69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="87.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="40">
+        <v>254</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="21" t="str">
+        <f>(RIGHT(D3,LEN(D3)-FIND(",",D3)))</f>
+        <v>8</v>
+      </c>
+      <c r="F3" s="21" t="str">
+        <f>B3 &amp;"/"&amp;(32-E3)</f>
+        <v>172.16.1.0/24</v>
+      </c>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="40">
+        <v>62</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="21" t="str">
+        <f t="shared" ref="E4:E13" si="0">(RIGHT(D4,LEN(D4)-FIND(",",D4)))</f>
+        <v>6</v>
+      </c>
+      <c r="F4" s="21" t="str">
+        <f t="shared" ref="F4:F13" si="1">B4 &amp;"/"&amp;(32-E4)</f>
+        <v>10.1.100.128/26</v>
+      </c>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="40">
+        <v>8190</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F5" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1.96.0/19</v>
+      </c>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="40">
+        <v>200</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F6" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="40">
+        <v>65000</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F7" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="40">
+        <v>2</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F8" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="40">
+        <v>4000</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F9" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="40">
+        <v>900</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F10" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="40">
+        <v>2200</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F11" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="40">
+        <v>16000</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F12" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="40">
+        <v>110</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="25" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="25" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="41"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="41">
+        <v>0</v>
+      </c>
+      <c r="C35" s="42">
+        <f>POWER(2,B35)</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="41" t="str">
+        <f>C35 &amp;"," &amp; B35</f>
+        <v>1,0</v>
+      </c>
+      <c r="E35" s="41"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="41">
+        <v>1</v>
+      </c>
+      <c r="C36" s="42">
+        <f t="shared" ref="C36:C67" si="2">POWER(2,B36)</f>
+        <v>2</v>
+      </c>
+      <c r="D36" s="41" t="str">
+        <f t="shared" ref="D36:D67" si="3">C36 &amp;"," &amp; B36</f>
+        <v>2,1</v>
+      </c>
+      <c r="E36" s="41"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="41">
+        <v>2</v>
+      </c>
+      <c r="C37" s="42">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D37" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>4,2</v>
+      </c>
+      <c r="E37" s="41"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="41">
+        <v>3</v>
+      </c>
+      <c r="C38" s="42">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D38" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>8,3</v>
+      </c>
+      <c r="E38" s="41"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="41">
+        <v>4</v>
+      </c>
+      <c r="C39" s="42">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D39" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>16,4</v>
+      </c>
+      <c r="E39" s="41"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="41">
+        <v>5</v>
+      </c>
+      <c r="C40" s="42">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="D40" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>32,5</v>
+      </c>
+      <c r="E40" s="41"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="41">
+        <v>6</v>
+      </c>
+      <c r="C41" s="42">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="D41" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>64,6</v>
+      </c>
+      <c r="E41" s="41"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="41">
+        <v>7</v>
+      </c>
+      <c r="C42" s="42">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="D42" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>128,7</v>
+      </c>
+      <c r="E42" s="41"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="41">
+        <v>8</v>
+      </c>
+      <c r="C43" s="42">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="D43" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>256,8</v>
+      </c>
+      <c r="E43" s="41"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="41">
+        <v>9</v>
+      </c>
+      <c r="C44" s="42">
+        <f t="shared" si="2"/>
+        <v>512</v>
+      </c>
+      <c r="D44" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>512,9</v>
+      </c>
+      <c r="E44" s="41"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="41">
+        <v>10</v>
+      </c>
+      <c r="C45" s="42">
+        <f t="shared" si="2"/>
+        <v>1024</v>
+      </c>
+      <c r="D45" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>1024,10</v>
+      </c>
+      <c r="E45" s="41"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="41">
+        <v>11</v>
+      </c>
+      <c r="C46" s="42">
+        <f t="shared" si="2"/>
+        <v>2048</v>
+      </c>
+      <c r="D46" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>2048,11</v>
+      </c>
+      <c r="E46" s="41"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="41">
+        <v>12</v>
+      </c>
+      <c r="C47" s="42">
+        <f t="shared" si="2"/>
+        <v>4096</v>
+      </c>
+      <c r="D47" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>4096,12</v>
+      </c>
+      <c r="E47" s="41"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="41">
+        <v>13</v>
+      </c>
+      <c r="C48" s="42">
+        <f t="shared" si="2"/>
+        <v>8192</v>
+      </c>
+      <c r="D48" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>8192,13</v>
+      </c>
+      <c r="E48" s="41"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="41">
+        <v>14</v>
+      </c>
+      <c r="C49" s="42">
+        <f t="shared" si="2"/>
+        <v>16384</v>
+      </c>
+      <c r="D49" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>16384,14</v>
+      </c>
+      <c r="E49" s="41"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="41">
+        <v>15</v>
+      </c>
+      <c r="C50" s="42">
+        <f t="shared" si="2"/>
+        <v>32768</v>
+      </c>
+      <c r="D50" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>32768,15</v>
+      </c>
+      <c r="E50" s="41"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="41">
+        <v>16</v>
+      </c>
+      <c r="C51" s="42">
+        <f t="shared" si="2"/>
+        <v>65536</v>
+      </c>
+      <c r="D51" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>65536,16</v>
+      </c>
+      <c r="E51" s="41"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="41">
+        <v>17</v>
+      </c>
+      <c r="C52" s="42">
+        <f t="shared" si="2"/>
+        <v>131072</v>
+      </c>
+      <c r="D52" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>131072,17</v>
+      </c>
+      <c r="E52" s="41"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="41">
+        <v>18</v>
+      </c>
+      <c r="C53" s="42">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+      <c r="D53" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>262144,18</v>
+      </c>
+      <c r="E53" s="41"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="41">
+        <v>19</v>
+      </c>
+      <c r="C54" s="42">
+        <f t="shared" si="2"/>
+        <v>524288</v>
+      </c>
+      <c r="D54" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>524288,19</v>
+      </c>
+      <c r="E54" s="41"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="41">
+        <v>20</v>
+      </c>
+      <c r="C55" s="42">
+        <f t="shared" si="2"/>
+        <v>1048576</v>
+      </c>
+      <c r="D55" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>1048576,20</v>
+      </c>
+      <c r="E55" s="41"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="41">
+        <v>21</v>
+      </c>
+      <c r="C56" s="42">
+        <f t="shared" si="2"/>
+        <v>2097152</v>
+      </c>
+      <c r="D56" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>2097152,21</v>
+      </c>
+      <c r="E56" s="41"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="41">
+        <v>22</v>
+      </c>
+      <c r="C57" s="42">
+        <f t="shared" si="2"/>
+        <v>4194304</v>
+      </c>
+      <c r="D57" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>4194304,22</v>
+      </c>
+      <c r="E57" s="41"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="41">
+        <v>23</v>
+      </c>
+      <c r="C58" s="42">
+        <f t="shared" si="2"/>
+        <v>8388608</v>
+      </c>
+      <c r="D58" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>8388608,23</v>
+      </c>
+      <c r="E58" s="41"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="41">
+        <v>24</v>
+      </c>
+      <c r="C59" s="42">
+        <f t="shared" si="2"/>
+        <v>16777216</v>
+      </c>
+      <c r="D59" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>16777216,24</v>
+      </c>
+      <c r="E59" s="41"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="41">
+        <v>25</v>
+      </c>
+      <c r="C60" s="42">
+        <f t="shared" si="2"/>
+        <v>33554432</v>
+      </c>
+      <c r="D60" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>33554432,25</v>
+      </c>
+      <c r="E60" s="41"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="41">
+        <v>26</v>
+      </c>
+      <c r="C61" s="42">
+        <f t="shared" si="2"/>
+        <v>67108864</v>
+      </c>
+      <c r="D61" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>67108864,26</v>
+      </c>
+      <c r="E61" s="41"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="41">
+        <v>27</v>
+      </c>
+      <c r="C62" s="42">
+        <f t="shared" si="2"/>
+        <v>134217728</v>
+      </c>
+      <c r="D62" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>134217728,27</v>
+      </c>
+      <c r="E62" s="41"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="41">
+        <v>28</v>
+      </c>
+      <c r="C63" s="42">
+        <f t="shared" si="2"/>
+        <v>268435456</v>
+      </c>
+      <c r="D63" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>268435456,28</v>
+      </c>
+      <c r="E63" s="41"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="41">
+        <v>29</v>
+      </c>
+      <c r="C64" s="42">
+        <f t="shared" si="2"/>
+        <v>536870912</v>
+      </c>
+      <c r="D64" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>536870912,29</v>
+      </c>
+      <c r="E64" s="41"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="41">
+        <v>30</v>
+      </c>
+      <c r="C65" s="42">
+        <f t="shared" si="2"/>
+        <v>1073741824</v>
+      </c>
+      <c r="D65" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>1073741824,30</v>
+      </c>
+      <c r="E65" s="41"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="41">
+        <v>31</v>
+      </c>
+      <c r="C66" s="42">
+        <f t="shared" si="2"/>
+        <v>2147483648</v>
+      </c>
+      <c r="D66" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>2147483648,31</v>
+      </c>
+      <c r="E66" s="41"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="41">
+        <v>32</v>
+      </c>
+      <c r="C67" s="42">
+        <f t="shared" si="2"/>
+        <v>4294967296</v>
+      </c>
+      <c r="D67" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>4294967296,32</v>
+      </c>
+      <c r="E67" s="41"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="41"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="41"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Host bits needed" prompt="Host bits selected must equal or exceed required hosts number." sqref="D3:D13" xr:uid="{7EBB5B15-C33A-40A0-9A0D-3B45F32E7BBE}">
+      <formula1>$D$34:$D$67</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2660,12 +3500,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2673,7 +3513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2682,7 +3522,7 @@
         <v>0.9999847412109375</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2691,7 +3531,7 @@
         <v>1.52587890625E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2700,7 +3540,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="16"/>
       <c r="C7" t="s">
         <v>25</v>
@@ -2715,28 +3555,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" customWidth="1"/>
-    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2776,7 +3616,7 @@
       <c r="N4" s="10"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>0</v>
       </c>
@@ -2814,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2837,7 +3677,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -2868,7 +3708,7 @@
       <c r="N7" s="11"/>
       <c r="O7" s="13"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -2899,7 +3739,7 @@
       <c r="N8" s="11"/>
       <c r="O8" s="13"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -2933,7 +3773,7 @@
       <c r="N9" s="11"/>
       <c r="O9" s="13"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -2967,13 +3807,13 @@
       <c r="N10" s="11"/>
       <c r="O10" s="13"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P12" s="16"/>
       <c r="Q12" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P13" s="16"/>
       <c r="Q13" s="14" t="s">
         <v>31</v>
@@ -2986,30 +3826,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5394DBD-56DF-4906-A928-C7277ECE51ED}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.109375" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3049,9 +3891,9 @@
       <c r="N4" s="10"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -3069,16 +3911,16 @@
         <v>1</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="12">
         <v>0</v>
       </c>
       <c r="K5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="12">
         <v>1</v>
@@ -3087,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3110,7 +3952,326 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <f>E5</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="11">
+        <f>IF(ISEVEN(SUM($B$7:$E$7)), 0, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
+        <f>F5</f>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f>IF(O7 =N7, 0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9">
+        <f>G5</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <f>H5</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <f>I5</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="11">
+        <f>IF(ISEVEN(SUM($B$8,$G$8:$I$8)), 0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="O8" s="13">
+        <f>J5</f>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f>IF(O8 =N8, 0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="9">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9">
+        <f>G5</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <f>H5</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="9">
+        <f>K5</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="11">
+        <f>IF(ISEVEN(SUM(C9:D9,G9:H9,K9)), 0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="13">
+        <f>L5</f>
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <f>IF(O9 =N9, 0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="9">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="9">
+        <f>E5</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9">
+        <f>G5</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="9">
+        <f>I5</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="9">
+        <f>K5</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="11">
+        <f>IF(ISEVEN(SUM(C10,E10,G10,I10,K10)), 0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <f>M5</f>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f>IF(O10 =N10, 0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12" t="str">
+        <f>IF(SUM(P7:P10) = 0, "No Error", "Yes, Error!")</f>
+        <v>Yes, Error!</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <f>BIN2DEC(P7&amp;P8&amp;P9&amp;P10)</f>
+        <v>12</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="12">
+        <v>1</v>
+      </c>
+      <c r="M5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -3141,7 +4302,7 @@
       <c r="N7" s="11"/>
       <c r="O7" s="13"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -3172,7 +4333,7 @@
       <c r="N8" s="11"/>
       <c r="O8" s="13"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -3206,7 +4367,7 @@
       <c r="N9" s="11"/>
       <c r="O9" s="13"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -3240,13 +4401,13 @@
       <c r="N10" s="11"/>
       <c r="O10" s="13"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P12" s="16"/>
       <c r="Q12" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P13" s="16"/>
       <c r="Q13" s="14" t="s">
         <v>31</v>
@@ -3258,7 +4419,328 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388C9215-712D-4A4A-97B9-0EC71221EA57}">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="12">
+        <v>1</v>
+      </c>
+      <c r="M5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <f>B5</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <f>E5</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="11">
+        <f>IF(ISEVEN(SUM($B$7:$E$7)), 0, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="O7" s="13">
+        <f>F5</f>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f>IF(O7 =N7, 0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <f>B5</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9">
+        <f>G5</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <f>I5</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="11">
+        <f>IF(ISEVEN(SUM($B$8,$G$8:$I$8)), 0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <f>J5</f>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f>IF(O8 =N8, 0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="9">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9">
+        <f>G5</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <f>H5</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="9">
+        <f>K5</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="11">
+        <f>IF(ISEVEN(SUM(C9:D9,G9:H9,K9)), 0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="13">
+        <f>L5</f>
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <f>IF(O9 =N9, 0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="9">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="9">
+        <f>E5</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9">
+        <f>G5</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="9">
+        <f>I5</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="9">
+        <f>K5</f>
+        <v>1</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="11">
+        <f>IF(ISEVEN(SUM(C10,E10,G10,I10,K10)), 0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <f>M5</f>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f>IF(O10 =N10, 0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12" t="str">
+        <f>IF(SUM(P7:P10) = 0, "No Error", "Yes, Error!")</f>
+        <v>No Error</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <f>BIN2DEC(P7&amp;P8&amp;P9&amp;P10)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F8FE82-F4C0-4C15-8B78-34F60311B7FE}">
   <dimension ref="A1:M14"/>
   <sheetViews>
@@ -3266,13 +4748,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3301,7 +4783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
       <c r="B2" s="21" t="s">
         <v>34</v>
@@ -3342,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -3351,7 +4833,7 @@
       </c>
       <c r="C3" s="23"/>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -3360,7 +4842,7 @@
       </c>
       <c r="C4" s="23"/>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -3369,7 +4851,7 @@
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="22">
         <v>4</v>
       </c>
@@ -3378,7 +4860,7 @@
       </c>
       <c r="C6" s="23"/>
     </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -3387,7 +4869,7 @@
       </c>
       <c r="C7" s="23"/>
     </row>
-    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="22">
         <v>6</v>
       </c>
@@ -3396,7 +4878,7 @@
       </c>
       <c r="C8" s="23"/>
     </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="22">
         <v>7</v>
       </c>
@@ -3405,7 +4887,7 @@
       </c>
       <c r="C9" s="23"/>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="22">
         <v>8</v>
       </c>
@@ -3414,7 +4896,7 @@
       </c>
       <c r="C10" s="23"/>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="22">
         <v>9</v>
       </c>
@@ -3423,7 +4905,7 @@
       </c>
       <c r="C11" s="23"/>
     </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="22">
         <v>10</v>
       </c>
@@ -3432,7 +4914,7 @@
       </c>
       <c r="C12" s="23"/>
     </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="22">
         <v>11</v>
       </c>
@@ -3441,7 +4923,7 @@
       </c>
       <c r="C13" s="23"/>
     </row>
-    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="22">
         <v>12</v>
       </c>
@@ -3457,7 +4939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A8069C-280C-46CF-9BC8-CAECB3D2297D}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -3465,19 +4947,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
       <c r="B2" s="21" t="s">
         <v>35</v>
@@ -3488,7 +4970,7 @@
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -3499,7 +4981,7 @@
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -3510,7 +4992,7 @@
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -3521,7 +5003,7 @@
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="22">
         <v>4</v>
       </c>
@@ -3532,7 +5014,7 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -3543,7 +5025,7 @@
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="22">
         <v>6</v>
       </c>
@@ -3554,7 +5036,7 @@
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="22">
         <v>7</v>
       </c>
@@ -3565,7 +5047,7 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="22">
         <v>8</v>
       </c>
@@ -3576,7 +5058,7 @@
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="22">
         <v>9</v>
       </c>
@@ -3587,7 +5069,7 @@
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="22">
         <v>10</v>
       </c>
@@ -3598,7 +5080,7 @@
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="22">
         <v>11</v>
       </c>
@@ -3609,7 +5091,7 @@
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="22">
         <v>12</v>
       </c>
@@ -3627,7 +5109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A99F657-2B68-4448-A74D-CBED5A27923E}">
   <dimension ref="A1:I55"/>
   <sheetViews>
@@ -3635,22 +5117,22 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.77734375" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="58.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
       <c r="B2" s="26" t="s">
         <v>38</v>
@@ -3667,7 +5149,7 @@
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -3687,7 +5169,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -3698,7 +5180,7 @@
       <c r="D4" s="30"/>
       <c r="E4" s="25"/>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -3709,7 +5191,7 @@
       <c r="D5" s="30"/>
       <c r="E5" s="25"/>
     </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="22">
         <v>4</v>
       </c>
@@ -3720,7 +5202,7 @@
       <c r="D6" s="30"/>
       <c r="E6" s="25"/>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -3731,7 +5213,7 @@
       <c r="D7" s="30"/>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="22">
         <v>6</v>
       </c>
@@ -3742,7 +5224,7 @@
       <c r="D8" s="30"/>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="22">
         <v>7</v>
       </c>
@@ -3753,7 +5235,7 @@
       <c r="D9" s="30"/>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="22">
         <v>8</v>
       </c>
@@ -3764,7 +5246,7 @@
       <c r="D10" s="30"/>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="22">
         <v>9</v>
       </c>
@@ -3775,7 +5257,7 @@
       <c r="D11" s="30"/>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="22">
         <v>10</v>
       </c>
@@ -3786,7 +5268,7 @@
       <c r="D12" s="30"/>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="22">
         <v>11</v>
       </c>
@@ -3797,7 +5279,7 @@
       <c r="D13" s="30"/>
       <c r="E13" s="25"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
         <v>53</v>
       </c>
@@ -3805,7 +5287,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>55</v>
       </c>
@@ -3813,17 +5295,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="33" t="s">
         <v>59</v>
       </c>
@@ -3834,7 +5316,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E24" s="34" t="s">
         <v>62</v>
       </c>
@@ -3845,7 +5327,7 @@
         <v>2147483646</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" s="36" t="s">
         <v>64</v>
       </c>
@@ -3856,7 +5338,7 @@
         <v>1073741822</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="34" t="s">
         <v>66</v>
       </c>
@@ -3867,7 +5349,7 @@
         <v>536870910</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E27" s="36" t="s">
         <v>68</v>
       </c>
@@ -3878,7 +5360,7 @@
         <v>268435454</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="34" t="s">
         <v>70</v>
       </c>
@@ -3889,7 +5371,7 @@
         <v>134217726</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="36" t="s">
         <v>72</v>
       </c>
@@ -3900,7 +5382,7 @@
         <v>67108862</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30" s="34" t="s">
         <v>74</v>
       </c>
@@ -3911,7 +5393,7 @@
         <v>33554430</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E31" s="34" t="s">
         <v>76</v>
       </c>
@@ -3922,7 +5404,7 @@
         <v>16777214</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E32" s="36" t="s">
         <v>78</v>
       </c>
@@ -3933,7 +5415,7 @@
         <v>8388606</v>
       </c>
     </row>
-    <row r="33" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E33" s="34" t="s">
         <v>80</v>
       </c>
@@ -3944,7 +5426,7 @@
         <v>4194302</v>
       </c>
     </row>
-    <row r="34" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E34" s="36" t="s">
         <v>82</v>
       </c>
@@ -3955,7 +5437,7 @@
         <v>2097150</v>
       </c>
     </row>
-    <row r="35" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E35" s="34" t="s">
         <v>84</v>
       </c>
@@ -3966,7 +5448,7 @@
         <v>1048574</v>
       </c>
     </row>
-    <row r="36" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E36" s="36" t="s">
         <v>86</v>
       </c>
@@ -3977,7 +5459,7 @@
         <v>524286</v>
       </c>
     </row>
-    <row r="37" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E37" s="34" t="s">
         <v>88</v>
       </c>
@@ -3988,7 +5470,7 @@
         <v>262142</v>
       </c>
     </row>
-    <row r="38" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E38" s="36" t="s">
         <v>90</v>
       </c>
@@ -3999,7 +5481,7 @@
         <v>131070</v>
       </c>
     </row>
-    <row r="39" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E39" s="36" t="s">
         <v>92</v>
       </c>
@@ -4010,7 +5492,7 @@
         <v>65534</v>
       </c>
     </row>
-    <row r="40" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E40" s="34" t="s">
         <v>94</v>
       </c>
@@ -4021,7 +5503,7 @@
         <v>32766</v>
       </c>
     </row>
-    <row r="41" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E41" s="36" t="s">
         <v>96</v>
       </c>
@@ -4032,7 +5514,7 @@
         <v>16382</v>
       </c>
     </row>
-    <row r="42" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E42" s="34" t="s">
         <v>98</v>
       </c>
@@ -4043,7 +5525,7 @@
         <v>8190</v>
       </c>
     </row>
-    <row r="43" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E43" s="36" t="s">
         <v>100</v>
       </c>
@@ -4054,7 +5536,7 @@
         <v>4094</v>
       </c>
     </row>
-    <row r="44" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E44" s="34" t="s">
         <v>102</v>
       </c>
@@ -4065,7 +5547,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="45" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E45" s="36" t="s">
         <v>104</v>
       </c>
@@ -4076,7 +5558,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="46" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E46" s="34" t="s">
         <v>106</v>
       </c>
@@ -4087,7 +5569,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="47" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="34" t="s">
         <v>108</v>
       </c>
@@ -4098,7 +5580,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E48" s="36" t="s">
         <v>110</v>
       </c>
@@ -4109,7 +5591,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E49" s="34" t="s">
         <v>112</v>
       </c>
@@ -4120,7 +5602,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E50" s="36" t="s">
         <v>114</v>
       </c>
@@ -4131,7 +5613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E51" s="34" t="s">
         <v>116</v>
       </c>
@@ -4142,7 +5624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E52" s="36" t="s">
         <v>118</v>
       </c>
@@ -4153,7 +5635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E53" s="34" t="s">
         <v>120</v>
       </c>
@@ -4164,7 +5646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E54" s="36" t="s">
         <v>122</v>
       </c>
@@ -4175,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E55" s="34" t="s">
         <v>124</v>
       </c>
@@ -4197,801 +5679,4 @@
   <drawing r:id="rId4"/>
   <legacyDrawing r:id="rId5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B349E9EF-46A3-44BF-ADBB-8103E35728F3}">
-  <dimension ref="A1:G69"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="87.21875" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="40">
-        <v>254</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="21" t="str">
-        <f>(RIGHT(D3,LEN(D3)-FIND(",",D3)))</f>
-        <v>8</v>
-      </c>
-      <c r="F3" s="21" t="str">
-        <f>B3 &amp;"/"&amp;(32-E3)</f>
-        <v>172.16.1.0/24</v>
-      </c>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="40">
-        <v>62</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="E4" s="21" t="str">
-        <f t="shared" ref="E4:E13" si="0">(RIGHT(D4,LEN(D4)-FIND(",",D4)))</f>
-        <v>6</v>
-      </c>
-      <c r="F4" s="21" t="str">
-        <f t="shared" ref="F4:F13" si="1">B4 &amp;"/"&amp;(32-E4)</f>
-        <v>10.1.100.128/26</v>
-      </c>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="40">
-        <v>8190</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F5" s="21" t="str">
-        <f t="shared" si="1"/>
-        <v>10.1.96.0/19</v>
-      </c>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="40">
-        <v>200</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E6" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F6" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="40">
-        <v>65000</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F7" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="40">
-        <v>2</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F8" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="40">
-        <v>4000</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E9" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F9" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="40">
-        <v>900</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F10" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" s="40">
-        <v>2200</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E11" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F11" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="40">
-        <v>16000</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F12" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="40">
-        <v>110</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="25" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F13" s="25" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E34" s="41"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="41">
-        <v>0</v>
-      </c>
-      <c r="C35" s="42">
-        <f>POWER(2,B35)</f>
-        <v>1</v>
-      </c>
-      <c r="D35" s="41" t="str">
-        <f>C35 &amp;"," &amp; B35</f>
-        <v>1,0</v>
-      </c>
-      <c r="E35" s="41"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="41">
-        <v>1</v>
-      </c>
-      <c r="C36" s="42">
-        <f t="shared" ref="C36:C67" si="2">POWER(2,B36)</f>
-        <v>2</v>
-      </c>
-      <c r="D36" s="41" t="str">
-        <f t="shared" ref="D36:D67" si="3">C36 &amp;"," &amp; B36</f>
-        <v>2,1</v>
-      </c>
-      <c r="E36" s="41"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="41">
-        <v>2</v>
-      </c>
-      <c r="C37" s="42">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="D37" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>4,2</v>
-      </c>
-      <c r="E37" s="41"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="41">
-        <v>3</v>
-      </c>
-      <c r="C38" s="42">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="D38" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>8,3</v>
-      </c>
-      <c r="E38" s="41"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="41">
-        <v>4</v>
-      </c>
-      <c r="C39" s="42">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="D39" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>16,4</v>
-      </c>
-      <c r="E39" s="41"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="41">
-        <v>5</v>
-      </c>
-      <c r="C40" s="42">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="D40" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>32,5</v>
-      </c>
-      <c r="E40" s="41"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="41">
-        <v>6</v>
-      </c>
-      <c r="C41" s="42">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
-      <c r="D41" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>64,6</v>
-      </c>
-      <c r="E41" s="41"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="41">
-        <v>7</v>
-      </c>
-      <c r="C42" s="42">
-        <f t="shared" si="2"/>
-        <v>128</v>
-      </c>
-      <c r="D42" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>128,7</v>
-      </c>
-      <c r="E42" s="41"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="41">
-        <v>8</v>
-      </c>
-      <c r="C43" s="42">
-        <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
-      <c r="D43" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>256,8</v>
-      </c>
-      <c r="E43" s="41"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="41">
-        <v>9</v>
-      </c>
-      <c r="C44" s="42">
-        <f t="shared" si="2"/>
-        <v>512</v>
-      </c>
-      <c r="D44" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>512,9</v>
-      </c>
-      <c r="E44" s="41"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="41">
-        <v>10</v>
-      </c>
-      <c r="C45" s="42">
-        <f t="shared" si="2"/>
-        <v>1024</v>
-      </c>
-      <c r="D45" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>1024,10</v>
-      </c>
-      <c r="E45" s="41"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="41">
-        <v>11</v>
-      </c>
-      <c r="C46" s="42">
-        <f t="shared" si="2"/>
-        <v>2048</v>
-      </c>
-      <c r="D46" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>2048,11</v>
-      </c>
-      <c r="E46" s="41"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="41">
-        <v>12</v>
-      </c>
-      <c r="C47" s="42">
-        <f t="shared" si="2"/>
-        <v>4096</v>
-      </c>
-      <c r="D47" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>4096,12</v>
-      </c>
-      <c r="E47" s="41"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="41">
-        <v>13</v>
-      </c>
-      <c r="C48" s="42">
-        <f t="shared" si="2"/>
-        <v>8192</v>
-      </c>
-      <c r="D48" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>8192,13</v>
-      </c>
-      <c r="E48" s="41"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="41">
-        <v>14</v>
-      </c>
-      <c r="C49" s="42">
-        <f t="shared" si="2"/>
-        <v>16384</v>
-      </c>
-      <c r="D49" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>16384,14</v>
-      </c>
-      <c r="E49" s="41"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="41">
-        <v>15</v>
-      </c>
-      <c r="C50" s="42">
-        <f t="shared" si="2"/>
-        <v>32768</v>
-      </c>
-      <c r="D50" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>32768,15</v>
-      </c>
-      <c r="E50" s="41"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="41">
-        <v>16</v>
-      </c>
-      <c r="C51" s="42">
-        <f t="shared" si="2"/>
-        <v>65536</v>
-      </c>
-      <c r="D51" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>65536,16</v>
-      </c>
-      <c r="E51" s="41"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="41">
-        <v>17</v>
-      </c>
-      <c r="C52" s="42">
-        <f t="shared" si="2"/>
-        <v>131072</v>
-      </c>
-      <c r="D52" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>131072,17</v>
-      </c>
-      <c r="E52" s="41"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="41">
-        <v>18</v>
-      </c>
-      <c r="C53" s="42">
-        <f t="shared" si="2"/>
-        <v>262144</v>
-      </c>
-      <c r="D53" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>262144,18</v>
-      </c>
-      <c r="E53" s="41"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="41">
-        <v>19</v>
-      </c>
-      <c r="C54" s="42">
-        <f t="shared" si="2"/>
-        <v>524288</v>
-      </c>
-      <c r="D54" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>524288,19</v>
-      </c>
-      <c r="E54" s="41"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="41">
-        <v>20</v>
-      </c>
-      <c r="C55" s="42">
-        <f t="shared" si="2"/>
-        <v>1048576</v>
-      </c>
-      <c r="D55" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>1048576,20</v>
-      </c>
-      <c r="E55" s="41"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="41">
-        <v>21</v>
-      </c>
-      <c r="C56" s="42">
-        <f t="shared" si="2"/>
-        <v>2097152</v>
-      </c>
-      <c r="D56" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>2097152,21</v>
-      </c>
-      <c r="E56" s="41"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="41">
-        <v>22</v>
-      </c>
-      <c r="C57" s="42">
-        <f t="shared" si="2"/>
-        <v>4194304</v>
-      </c>
-      <c r="D57" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>4194304,22</v>
-      </c>
-      <c r="E57" s="41"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="41">
-        <v>23</v>
-      </c>
-      <c r="C58" s="42">
-        <f t="shared" si="2"/>
-        <v>8388608</v>
-      </c>
-      <c r="D58" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>8388608,23</v>
-      </c>
-      <c r="E58" s="41"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="41">
-        <v>24</v>
-      </c>
-      <c r="C59" s="42">
-        <f t="shared" si="2"/>
-        <v>16777216</v>
-      </c>
-      <c r="D59" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>16777216,24</v>
-      </c>
-      <c r="E59" s="41"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="41">
-        <v>25</v>
-      </c>
-      <c r="C60" s="42">
-        <f t="shared" si="2"/>
-        <v>33554432</v>
-      </c>
-      <c r="D60" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>33554432,25</v>
-      </c>
-      <c r="E60" s="41"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="41">
-        <v>26</v>
-      </c>
-      <c r="C61" s="42">
-        <f t="shared" si="2"/>
-        <v>67108864</v>
-      </c>
-      <c r="D61" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>67108864,26</v>
-      </c>
-      <c r="E61" s="41"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="41">
-        <v>27</v>
-      </c>
-      <c r="C62" s="42">
-        <f t="shared" si="2"/>
-        <v>134217728</v>
-      </c>
-      <c r="D62" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>134217728,27</v>
-      </c>
-      <c r="E62" s="41"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="41">
-        <v>28</v>
-      </c>
-      <c r="C63" s="42">
-        <f t="shared" si="2"/>
-        <v>268435456</v>
-      </c>
-      <c r="D63" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>268435456,28</v>
-      </c>
-      <c r="E63" s="41"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" s="41">
-        <v>29</v>
-      </c>
-      <c r="C64" s="42">
-        <f t="shared" si="2"/>
-        <v>536870912</v>
-      </c>
-      <c r="D64" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>536870912,29</v>
-      </c>
-      <c r="E64" s="41"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B65" s="41">
-        <v>30</v>
-      </c>
-      <c r="C65" s="42">
-        <f t="shared" si="2"/>
-        <v>1073741824</v>
-      </c>
-      <c r="D65" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>1073741824,30</v>
-      </c>
-      <c r="E65" s="41"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" s="41">
-        <v>31</v>
-      </c>
-      <c r="C66" s="42">
-        <f t="shared" si="2"/>
-        <v>2147483648</v>
-      </c>
-      <c r="D66" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>2147483648,31</v>
-      </c>
-      <c r="E66" s="41"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="41">
-        <v>32</v>
-      </c>
-      <c r="C67" s="42">
-        <f t="shared" si="2"/>
-        <v>4294967296</v>
-      </c>
-      <c r="D67" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>4294967296,32</v>
-      </c>
-      <c r="E67" s="41"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="41"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="41"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B69" s="41"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="41"/>
-      <c r="E69" s="41"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Host bits needed" prompt="Host bits selected must equal or exceed required hosts number." sqref="D3:D13" xr:uid="{7EBB5B15-C33A-40A0-9A0D-3B45F32E7BBE}">
-      <formula1>$D$34:$D$67</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>